<commit_message>
Refactored possibilities marker. Added markings for all directions.
</commit_message>
<xml_diff>
--- a/doc/reversi_board.xlsx
+++ b/doc/reversi_board.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marius.crisan.RO\workspace\CppKata\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Documents\workspace\CppKata\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
   <si>
     <t>B</t>
   </si>
@@ -115,7 +115,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -130,13 +130,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -419,7 +412,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +481,9 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -506,9 +501,7 @@
       <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -523,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -540,7 +533,9 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>

</xml_diff>